<commit_message>
add predict_cost to boors.py
</commit_message>
<xml_diff>
--- a/database/industries/folad/fakhouz/product/monthly.xlsx
+++ b/database/industries/folad/fakhouz/product/monthly.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\EBRAHIMI\Desktop\Trade\database\industries\folad\fakhouz\product\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\folad\fakhouz\product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8F7A97-672F-48BF-8950-6A881FD44CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="82">
   <si>
     <t>Pouya Finance</t>
   </si>
@@ -208,9 +207,6 @@
     <t>اسلب داخلی</t>
   </si>
   <si>
-    <t>بلوم ، بیلت</t>
-  </si>
-  <si>
     <t>ورق</t>
   </si>
   <si>
@@ -274,7 +270,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -746,10 +742,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BB87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2215,7 +2213,7 @@
     </row>
     <row r="16" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>56</v>
@@ -2374,7 +2372,7 @@
     </row>
     <row r="17" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>56</v>
@@ -2533,7 +2531,7 @@
     </row>
     <row r="18" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>56</v>
@@ -2692,7 +2690,7 @@
     </row>
     <row r="19" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>56</v>
@@ -2851,7 +2849,7 @@
     </row>
     <row r="20" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>56</v>
@@ -3010,7 +3008,7 @@
     </row>
     <row r="21" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>56</v>
@@ -3169,7 +3167,7 @@
     </row>
     <row r="22" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -3226,7 +3224,7 @@
     </row>
     <row r="23" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B23" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -3383,7 +3381,7 @@
     </row>
     <row r="24" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
@@ -3705,7 +3703,7 @@
     </row>
     <row r="28" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -3917,7 +3915,7 @@
     </row>
     <row r="30" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -4769,7 +4767,7 @@
     </row>
     <row r="36" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>56</v>
@@ -4928,7 +4926,7 @@
     </row>
     <row r="37" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>56</v>
@@ -5087,7 +5085,7 @@
     </row>
     <row r="38" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>56</v>
@@ -5246,7 +5244,7 @@
     </row>
     <row r="39" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>56</v>
@@ -5405,7 +5403,7 @@
     </row>
     <row r="40" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B40" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>56</v>
@@ -5564,7 +5562,7 @@
     </row>
     <row r="41" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>56</v>
@@ -5723,7 +5721,7 @@
     </row>
     <row r="42" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="15"/>
@@ -5780,7 +5778,7 @@
     </row>
     <row r="43" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B43" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
@@ -5937,7 +5935,7 @@
     </row>
     <row r="44" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
@@ -5994,7 +5992,7 @@
     </row>
     <row r="45" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B45" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
@@ -6151,7 +6149,7 @@
     </row>
     <row r="46" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
@@ -6473,7 +6471,7 @@
     </row>
     <row r="50" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -6685,7 +6683,7 @@
     </row>
     <row r="52" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
@@ -6745,7 +6743,7 @@
         <v>55</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D53" s="11"/>
       <c r="E53" s="11">
@@ -6904,7 +6902,7 @@
         <v>58</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D54" s="13"/>
       <c r="E54" s="13" t="s">
@@ -7063,7 +7061,7 @@
         <v>59</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="11" t="s">
@@ -7222,7 +7220,7 @@
         <v>60</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D56" s="13"/>
       <c r="E56" s="13">
@@ -7381,7 +7379,7 @@
         <v>61</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D57" s="11"/>
       <c r="E57" s="11">
@@ -7537,10 +7535,10 @@
     </row>
     <row r="58" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B58" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D58" s="13"/>
       <c r="E58" s="13" t="s">
@@ -7696,10 +7694,10 @@
     </row>
     <row r="59" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D59" s="11"/>
       <c r="E59" s="11" t="s">
@@ -7855,10 +7853,10 @@
     </row>
     <row r="60" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B60" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D60" s="13"/>
       <c r="E60" s="13">
@@ -8014,10 +8012,10 @@
     </row>
     <row r="61" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B61" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D61" s="11"/>
       <c r="E61" s="11">
@@ -8173,10 +8171,10 @@
     </row>
     <row r="62" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B62" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D62" s="13"/>
       <c r="E62" s="13" t="s">
@@ -8332,10 +8330,10 @@
     </row>
     <row r="63" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B63" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D63" s="11"/>
       <c r="E63" s="11" t="s">
@@ -8491,7 +8489,7 @@
     </row>
     <row r="64" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B64" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
@@ -8548,10 +8546,10 @@
     </row>
     <row r="65" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B65" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D65" s="17"/>
       <c r="E65" s="17" t="s">
@@ -8707,7 +8705,7 @@
     </row>
     <row r="66" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B66" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
@@ -8764,10 +8762,10 @@
     </row>
     <row r="67" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D67" s="17"/>
       <c r="E67" s="17" t="s">
@@ -8923,7 +8921,7 @@
     </row>
     <row r="68" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
@@ -8980,10 +8978,10 @@
     </row>
     <row r="69" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D69" s="11"/>
       <c r="E69" s="11" t="s">
@@ -9139,7 +9137,7 @@
     </row>
     <row r="70" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B70" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="19"/>
@@ -9461,7 +9459,7 @@
     </row>
     <row r="74" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B74" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
@@ -9673,7 +9671,7 @@
     </row>
     <row r="76" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B76" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
@@ -9733,7 +9731,7 @@
         <v>55</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D77" s="11"/>
       <c r="E77" s="11">
@@ -9892,7 +9890,7 @@
         <v>58</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="13" t="s">
@@ -10051,7 +10049,7 @@
         <v>59</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D79" s="11"/>
       <c r="E79" s="11" t="s">
@@ -10210,7 +10208,7 @@
         <v>60</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="13">
@@ -10369,7 +10367,7 @@
         <v>61</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D81" s="11"/>
       <c r="E81" s="11">
@@ -10525,10 +10523,10 @@
     </row>
     <row r="82" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B82" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D82" s="13"/>
       <c r="E82" s="13" t="s">
@@ -10684,10 +10682,10 @@
     </row>
     <row r="83" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B83" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D83" s="11"/>
       <c r="E83" s="11" t="s">
@@ -10843,10 +10841,10 @@
     </row>
     <row r="84" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B84" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="13">
@@ -11002,10 +11000,10 @@
     </row>
     <row r="85" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B85" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D85" s="11"/>
       <c r="E85" s="11">
@@ -11161,10 +11159,10 @@
     </row>
     <row r="86" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B86" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="13" t="s">
@@ -11320,10 +11318,10 @@
     </row>
     <row r="87" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B87" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D87" s="11"/>
       <c r="E87" s="11" t="s">

</xml_diff>